<commit_message>
modified:   CODE/EDA.ipynb 	new file:   "CODE/\352\267\274\354\240\221\354\240\220\353\247\244\354\271\255.ipynb" 	modified:   "CODE/\353\217\204\353\241\234\352\265\254\354\241\260_\353\263\221\355\225\251.ipynb" 	modified:   "INFO/\353\252\250\353\215\270\352\262\200\354\246\235_\353\263\200\354\210\230\353\263\204.xlsx"
</commit_message>
<xml_diff>
--- a/INFO/모델검증_변수별.xlsx
+++ b/INFO/모델검증_변수별.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\모델검증\INFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6346B8ED-B78C-4792-86AF-9C609EF76835}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A49DCF4-7C90-4B97-AFCB-3EAED54B8DC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="27840" windowHeight="12765" xr2:uid="{AEEB1354-AAD5-486B-B36A-393DB3914176}"/>
+    <workbookView xWindow="13440" yWindow="0" windowWidth="27840" windowHeight="12765" xr2:uid="{AEEB1354-AAD5-486B-B36A-393DB3914176}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="49">
   <si>
     <t>org</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -188,11 +188,27 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>z</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
+    <t>ROAD_RANK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHR1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHR2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHR3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHR4</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -255,12 +271,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -577,15 +596,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353AEE09-F6FB-4870-B029-D81A8987889A}">
-  <dimension ref="B1:AK53"/>
+  <dimension ref="A1:AL53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AF10" sqref="AF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:38" x14ac:dyDescent="0.3">
       <c r="S1">
         <v>0</v>
       </c>
@@ -602,7 +621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -627,23 +646,11 @@
       <c r="W2" t="s">
         <v>42</v>
       </c>
-      <c r="AE2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="Y2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -698,17 +705,44 @@
       <c r="W3" t="s">
         <v>3</v>
       </c>
+      <c r="Y3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>3</v>
+      </c>
       <c r="AF3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="AG3" t="s">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>4</v>
       </c>
       <c r="AK3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:37" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>26</v>
       </c>
@@ -763,11 +797,47 @@
       <c r="W4">
         <v>0.87863076664009299</v>
       </c>
-      <c r="AK4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="Y4">
+        <v>102</v>
+      </c>
+      <c r="Z4">
+        <v>14.458342377310901</v>
+      </c>
+      <c r="AA4">
+        <v>0.79427826686207703</v>
+      </c>
+      <c r="AB4">
+        <v>19.176037796887801</v>
+      </c>
+      <c r="AC4">
+        <v>20.8524299239761</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>0.91380409331349199</v>
+      </c>
+      <c r="AF4">
+        <v>102</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>5.7398633715288101</v>
+      </c>
+      <c r="AH4">
+        <v>9.7273490330987702</v>
+      </c>
+      <c r="AI4">
+        <v>12.040136804132899</v>
+      </c>
+      <c r="AJ4">
+        <v>9.6260122190623196</v>
+      </c>
+      <c r="AK4">
+        <v>10.1436415515671</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>27</v>
       </c>
@@ -822,8 +892,44 @@
       <c r="W5">
         <v>26.4041135977244</v>
       </c>
-    </row>
-    <row r="6" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="Y5">
+        <v>102</v>
+      </c>
+      <c r="Z5">
+        <v>6.2979392553440503</v>
+      </c>
+      <c r="AA5">
+        <v>25.353831756336199</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>3.9378389869533601</v>
+      </c>
+      <c r="AC5">
+        <v>4.1309765886275196</v>
+      </c>
+      <c r="AD5">
+        <v>26.008245347754301</v>
+      </c>
+      <c r="AF5">
+        <v>107</v>
+      </c>
+      <c r="AG5">
+        <v>25.3462850378761</v>
+      </c>
+      <c r="AH5">
+        <v>0.74360342834137305</v>
+      </c>
+      <c r="AI5">
+        <v>38.044222498169901</v>
+      </c>
+      <c r="AJ5">
+        <v>28.438996653996401</v>
+      </c>
+      <c r="AK5" s="1">
+        <v>0.454417739294115</v>
+      </c>
+    </row>
+    <row r="6" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>19</v>
       </c>
@@ -878,8 +984,45 @@
       <c r="W6">
         <v>17.6559602051383</v>
       </c>
-    </row>
-    <row r="7" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="Y6">
+        <v>102</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>2.9488555926639402</v>
+      </c>
+      <c r="AA6">
+        <v>14.5297598477938</v>
+      </c>
+      <c r="AB6">
+        <v>11.4226431282479</v>
+      </c>
+      <c r="AC6">
+        <v>3.7408005392025898</v>
+      </c>
+      <c r="AD6">
+        <v>18.3931600321114</v>
+      </c>
+      <c r="AE6" s="2"/>
+      <c r="AF6">
+        <v>103</v>
+      </c>
+      <c r="AG6">
+        <v>17.695228834457701</v>
+      </c>
+      <c r="AH6">
+        <v>0.20620366956127001</v>
+      </c>
+      <c r="AI6">
+        <v>32.175858123390398</v>
+      </c>
+      <c r="AJ6">
+        <v>23.783799749203101</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>0.19056345793315199</v>
+      </c>
+    </row>
+    <row r="7" spans="2:38" x14ac:dyDescent="0.3">
       <c r="R7">
         <v>1</v>
       </c>
@@ -898,8 +1041,26 @@
       <c r="W7">
         <v>3.9649901259539702</v>
       </c>
-    </row>
-    <row r="8" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="AF7">
+        <v>105</v>
+      </c>
+      <c r="AG7">
+        <v>26.400565007696699</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>0.37951848471095201</v>
+      </c>
+      <c r="AI7">
+        <v>31.977580927658</v>
+      </c>
+      <c r="AJ7">
+        <v>23.646340259218899</v>
+      </c>
+      <c r="AK7">
+        <v>0.38046018867733</v>
+      </c>
+    </row>
+    <row r="8" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -954,8 +1115,44 @@
       <c r="W8">
         <v>0.23958274871382301</v>
       </c>
-    </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="Y8" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF8">
+        <v>106</v>
+      </c>
+      <c r="AG8">
+        <v>17.973778702410701</v>
+      </c>
+      <c r="AH8">
+        <v>0.61148398279761895</v>
+      </c>
+      <c r="AI8">
+        <v>38.205302154454699</v>
+      </c>
+      <c r="AJ8">
+        <v>28.309953947662901</v>
+      </c>
+      <c r="AK8" s="1">
+        <v>0.31197688083988001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>19</v>
       </c>
@@ -1010,8 +1207,26 @@
       <c r="W9">
         <v>2.3200363528160599</v>
       </c>
-    </row>
-    <row r="10" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="Y9">
+        <v>102</v>
+      </c>
+      <c r="Z9">
+        <v>2.0254119655249299</v>
+      </c>
+      <c r="AA9">
+        <v>1.7721264258023299</v>
+      </c>
+      <c r="AB9">
+        <v>51.775160979322798</v>
+      </c>
+      <c r="AC9">
+        <v>19.681002116677298</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>0.89554729756941998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:38" x14ac:dyDescent="0.3">
       <c r="R10">
         <v>2</v>
       </c>
@@ -1030,8 +1245,26 @@
       <c r="W10">
         <v>16.151129063124799</v>
       </c>
-    </row>
-    <row r="11" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="AF10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -1086,14 +1319,44 @@
       <c r="W11">
         <v>1.2959662841008399</v>
       </c>
+      <c r="Y11" t="s">
+        <v>32</v>
+      </c>
       <c r="Z11" t="s">
-        <v>43</v>
+        <v>0</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>1</v>
       </c>
       <c r="AB11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="2:37" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>9.4653634620468008</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>7.9211258923028103</v>
+      </c>
+      <c r="AI11">
+        <v>17.185845173230199</v>
+      </c>
+      <c r="AJ11">
+        <v>13.280546689028</v>
+      </c>
+      <c r="AK11">
+        <v>8.1797113086552304</v>
+      </c>
+    </row>
+    <row r="12" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>19</v>
       </c>
@@ -1148,8 +1411,44 @@
       <c r="W12">
         <v>31.355048616449899</v>
       </c>
-    </row>
-    <row r="13" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="Y12">
+        <v>102</v>
+      </c>
+      <c r="Z12">
+        <v>7.5983016315432197</v>
+      </c>
+      <c r="AA12">
+        <v>9.2533968634159205</v>
+      </c>
+      <c r="AB12">
+        <v>67.589271184504298</v>
+      </c>
+      <c r="AC12">
+        <v>32.903491616417298</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>6.8773555732527196</v>
+      </c>
+      <c r="AF12">
+        <v>3</v>
+      </c>
+      <c r="AG12">
+        <v>9.3023980499119201</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>8.8478862355819707</v>
+      </c>
+      <c r="AI12">
+        <v>13.4012372561007</v>
+      </c>
+      <c r="AJ12">
+        <v>12.612142078501099</v>
+      </c>
+      <c r="AK12">
+        <v>9.5340644813405504</v>
+      </c>
+    </row>
+    <row r="13" spans="2:38" x14ac:dyDescent="0.3">
       <c r="J13">
         <v>17</v>
       </c>
@@ -1186,8 +1485,26 @@
       <c r="W13">
         <v>36.394333382554002</v>
       </c>
-    </row>
-    <row r="14" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="AF13">
+        <v>2</v>
+      </c>
+      <c r="AG13">
+        <v>16.080048265593501</v>
+      </c>
+      <c r="AH13" s="1">
+        <v>2.7055790625438401</v>
+      </c>
+      <c r="AI13">
+        <v>29.645773178885701</v>
+      </c>
+      <c r="AJ13">
+        <v>22.129939952841401</v>
+      </c>
+      <c r="AK13">
+        <v>3.05353758560643</v>
+      </c>
+    </row>
+    <row r="14" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -1206,8 +1523,44 @@
       <c r="G14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="Y14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF14">
+        <v>1</v>
+      </c>
+      <c r="AG14">
+        <v>21.175498168549399</v>
+      </c>
+      <c r="AH14">
+        <v>1.39470176134436</v>
+      </c>
+      <c r="AI14">
+        <v>41.945759746712099</v>
+      </c>
+      <c r="AJ14">
+        <v>30.348620446724102</v>
+      </c>
+      <c r="AK14" s="1">
+        <v>1.0775070232485999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>26</v>
       </c>
@@ -1265,8 +1618,26 @@
       <c r="W15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="Y15">
+        <v>102</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>2.3386136613357902</v>
+      </c>
+      <c r="AA15">
+        <v>7.6910508583755197</v>
+      </c>
+      <c r="AB15">
+        <v>6.5597753453247796</v>
+      </c>
+      <c r="AC15">
+        <v>8.7592843196691295</v>
+      </c>
+      <c r="AD15">
+        <v>7.7659904950297998</v>
+      </c>
+    </row>
+    <row r="16" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>27</v>
       </c>
@@ -1321,8 +1692,26 @@
       <c r="W16" s="1">
         <v>0.89490886519816204</v>
       </c>
-    </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y16">
+        <v>102</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>3.4911369401763701</v>
+      </c>
+      <c r="AA16">
+        <v>15.960281272362501</v>
+      </c>
+      <c r="AB16">
+        <v>5.4294382382340602</v>
+      </c>
+      <c r="AC16">
+        <v>6.6389934518103404</v>
+      </c>
+      <c r="AD16">
+        <v>16.181856670176</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>19</v>
       </c>
@@ -1377,8 +1766,26 @@
       <c r="W17" s="1">
         <v>0.95507271576332597</v>
       </c>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y17">
+        <v>102</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>4.2177249447826899</v>
+      </c>
+      <c r="AA17">
+        <v>8.1951636465825199</v>
+      </c>
+      <c r="AB17">
+        <v>8.3039307877153306</v>
+      </c>
+      <c r="AC17">
+        <v>7.9376309037467001</v>
+      </c>
+      <c r="AD17">
+        <v>8.8858861397525697</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>17</v>
       </c>
@@ -1415,8 +1822,26 @@
       <c r="O18">
         <v>8.2550185122963207</v>
       </c>
-    </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y18">
+        <v>102</v>
+      </c>
+      <c r="Z18">
+        <v>9.29262227525669</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>4.7416957455094497</v>
+      </c>
+      <c r="AB18">
+        <v>10.8875425381733</v>
+      </c>
+      <c r="AC18">
+        <v>12.336197681233401</v>
+      </c>
+      <c r="AD18">
+        <v>5.0086232313124501</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>18</v>
       </c>
@@ -1453,8 +1878,26 @@
       <c r="W19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y19">
+        <v>102</v>
+      </c>
+      <c r="Z19">
+        <v>11.780149353861299</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>2.9805541815858998</v>
+      </c>
+      <c r="AB19">
+        <v>15.145707981469201</v>
+      </c>
+      <c r="AC19">
+        <v>10.0477763391984</v>
+      </c>
+      <c r="AD19">
+        <v>3.9429270492364301</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
       <c r="J20" t="s">
         <v>5</v>
       </c>
@@ -1492,7 +1935,7 @@
         <v>6.8773555732527196</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>5</v>
       </c>
@@ -1529,8 +1972,26 @@
       <c r="O21">
         <v>3.77416323968552</v>
       </c>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y21" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>20</v>
       </c>
@@ -1567,8 +2028,26 @@
       <c r="W22" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y22">
+        <v>102</v>
+      </c>
+      <c r="Z22">
+        <v>16.355045286116301</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>2.8549644978870101</v>
+      </c>
+      <c r="AB22">
+        <v>14.8314796990303</v>
+      </c>
+      <c r="AC22">
+        <v>10.1526197254504</v>
+      </c>
+      <c r="AD22">
+        <v>3.77416323968552</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
       <c r="J23" t="s">
         <v>6</v>
       </c>
@@ -1609,7 +2088,7 @@
         <v>7.8131274115434701</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -1664,8 +2143,26 @@
       <c r="W24">
         <v>16.268728088842799</v>
       </c>
-    </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y24" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>20</v>
       </c>
@@ -1702,8 +2199,26 @@
       <c r="W25">
         <v>9.14343917070779</v>
       </c>
-    </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y25">
+        <v>107</v>
+      </c>
+      <c r="Z25">
+        <v>41.453686400551902</v>
+      </c>
+      <c r="AA25">
+        <v>0.58467415439386405</v>
+      </c>
+      <c r="AB25">
+        <v>37.022757142535397</v>
+      </c>
+      <c r="AC25">
+        <v>27.3234474922365</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>0.34200609095417001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>15</v>
       </c>
@@ -1747,7 +2262,7 @@
         <v>5.1113099860893199</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>20</v>
       </c>
@@ -1802,8 +2317,26 @@
       <c r="W27">
         <v>3.9686127994846898</v>
       </c>
-    </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y27" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>7</v>
       </c>
@@ -1858,8 +2391,26 @@
       <c r="W28">
         <v>6.0447475679321503</v>
       </c>
-    </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y28">
+        <v>107</v>
+      </c>
+      <c r="Z28">
+        <v>20.249193588544401</v>
+      </c>
+      <c r="AA28">
+        <v>0.62752111080789896</v>
+      </c>
+      <c r="AB28">
+        <v>36.240524644697501</v>
+      </c>
+      <c r="AC28">
+        <v>26.859311805595301</v>
+      </c>
+      <c r="AD28" s="1">
+        <v>0.42950019548942397</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>20</v>
       </c>
@@ -1897,7 +2448,7 @@
         <v>10.687957841817299</v>
       </c>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>8</v>
       </c>
@@ -1937,8 +2488,26 @@
       <c r="W30">
         <v>4.6269223740522003</v>
       </c>
-    </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y30" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>20</v>
       </c>
@@ -1993,8 +2562,26 @@
       <c r="W31">
         <v>3.1064733452075899</v>
       </c>
-    </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y31">
+        <v>107</v>
+      </c>
+      <c r="Z31">
+        <v>19.4780787096003</v>
+      </c>
+      <c r="AA31">
+        <v>0.96927563044505805</v>
+      </c>
+      <c r="AB31">
+        <v>40.390414041604203</v>
+      </c>
+      <c r="AC31">
+        <v>30.913839927506199</v>
+      </c>
+      <c r="AD31" s="1">
+        <v>0.56294034468131804</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.3">
       <c r="J32" t="s">
         <v>8</v>
       </c>
@@ -2016,8 +2603,26 @@
       <c r="W32">
         <v>2.8606678416609599</v>
       </c>
-    </row>
-    <row r="33" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="Y32">
+        <v>103</v>
+      </c>
+      <c r="Z32">
+        <v>17.695228834457701</v>
+      </c>
+      <c r="AA32">
+        <v>0.20620366956127001</v>
+      </c>
+      <c r="AB32">
+        <v>32.175858123390398</v>
+      </c>
+      <c r="AC32">
+        <v>23.783799749203101</v>
+      </c>
+      <c r="AD32" s="1">
+        <v>0.19056345793315199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J33">
         <v>1</v>
       </c>
@@ -2036,13 +2641,31 @@
       <c r="O33" s="1">
         <v>0.40704314110287299</v>
       </c>
-    </row>
-    <row r="34" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="Y33">
+        <v>105</v>
+      </c>
+      <c r="Z33">
+        <v>26.400565007696699</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>0.37951848471095201</v>
+      </c>
+      <c r="AB33">
+        <v>31.977580927658</v>
+      </c>
+      <c r="AC33">
+        <v>23.646340259218899</v>
+      </c>
+      <c r="AD33">
+        <v>0.38046018867733</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="R34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="10:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
       <c r="R35">
         <v>0</v>
       </c>
@@ -2061,8 +2684,26 @@
       <c r="W35">
         <v>3.7344957386381901</v>
       </c>
-    </row>
-    <row r="36" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="Y35" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
       <c r="R36">
         <v>2</v>
       </c>
@@ -2081,13 +2722,49 @@
       <c r="W36">
         <v>3.9624059159443701</v>
       </c>
-    </row>
-    <row r="37" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="Y36">
+        <v>106</v>
+      </c>
+      <c r="Z36">
+        <v>17.973778702410701</v>
+      </c>
+      <c r="AA36">
+        <v>0.61148398279761895</v>
+      </c>
+      <c r="AB36">
+        <v>38.205302154454699</v>
+      </c>
+      <c r="AC36">
+        <v>28.309953947662901</v>
+      </c>
+      <c r="AD36" s="1">
+        <v>0.31197688083988001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
       <c r="K37" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="38" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="Y37">
+        <v>107</v>
+      </c>
+      <c r="Z37">
+        <v>24.357183170064001</v>
+      </c>
+      <c r="AA37">
+        <v>0.88381760322373004</v>
+      </c>
+      <c r="AB37">
+        <v>39.997622593039097</v>
+      </c>
+      <c r="AC37">
+        <v>29.866886530298299</v>
+      </c>
+      <c r="AD37" s="1">
+        <v>0.50016986438729605</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
       <c r="K38" t="s">
         <v>18</v>
       </c>
@@ -2095,7 +2772,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="10:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
       <c r="R39">
         <v>0</v>
       </c>
@@ -2115,12 +2792,12 @@
         <v>0.34200609095417001</v>
       </c>
     </row>
-    <row r="41" spans="10:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
       <c r="R41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="10:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
       <c r="R42">
         <v>0</v>
       </c>
@@ -2140,7 +2817,7 @@
         <v>0.41249388833559197</v>
       </c>
     </row>
-    <row r="43" spans="10:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
       <c r="R43">
         <v>2</v>
       </c>
@@ -2160,12 +2837,12 @@
         <v>0.54766268217693304</v>
       </c>
     </row>
-    <row r="45" spans="10:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
       <c r="R45" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="10:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
       <c r="R46">
         <v>0</v>
       </c>
@@ -2185,7 +2862,7 @@
         <v>0.42765635013352299</v>
       </c>
     </row>
-    <row r="47" spans="10:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
       <c r="R47">
         <v>1</v>
       </c>
@@ -2205,7 +2882,22 @@
         <v>1.1871858708518599</v>
       </c>
     </row>
-    <row r="48" spans="10:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" t="s">
+        <v>24</v>
+      </c>
       <c r="R48">
         <v>2</v>
       </c>
@@ -2225,7 +2917,16 @@
         <v>1.3034712763496401</v>
       </c>
     </row>
-    <row r="49" spans="18:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" t="s">
+        <v>29</v>
+      </c>
+      <c r="G49" t="s">
+        <v>25</v>
+      </c>
       <c r="R49">
         <v>3</v>
       </c>
@@ -2245,12 +2946,17 @@
         <v>0.501112459852047</v>
       </c>
     </row>
-    <row r="51" spans="18:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="G50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="2:23" x14ac:dyDescent="0.3">
       <c r="R51" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="18:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:23" x14ac:dyDescent="0.3">
       <c r="R52">
         <v>0</v>
       </c>
@@ -2270,7 +2976,7 @@
         <v>0.39120857127196801</v>
       </c>
     </row>
-    <row r="53" spans="18:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:23" x14ac:dyDescent="0.3">
       <c r="R53">
         <v>1</v>
       </c>

</xml_diff>